<commit_message>
added task 9 files to TASK 9 folder
</commit_message>
<xml_diff>
--- a/Work History.xlsx
+++ b/Work History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fusion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0EF8D9-2C1C-4CD5-8ADC-255DCE536D06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B573C1EC-D718-4D73-AD1A-ACE73ED2CD1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7185" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -330,7 +330,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mmm"/>
-    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -559,10 +559,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -602,13 +602,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>107675</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>78441</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3898624</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>99104</xdr:rowOff>
+      <xdr:rowOff>177545</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -637,7 +637,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1441175" y="5905500"/>
+          <a:off x="1441175" y="7720853"/>
           <a:ext cx="3790949" cy="2004104"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1147,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
added TASk-9 output-pdf,template,report catalog files
</commit_message>
<xml_diff>
--- a/Work History.xlsx
+++ b/Work History.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fusion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B573C1EC-D718-4D73-AD1A-ACE73ED2CD1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EE11CD-C585-489C-A1B1-5D29EBE79CE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7185" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DAILY-TRACKER" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
   <si>
     <r>
       <rPr>
@@ -306,9 +306,6 @@
     <t>AP Aging Report</t>
   </si>
   <si>
-    <t>TASK 11</t>
-  </si>
-  <si>
     <t>TASK12</t>
   </si>
   <si>
@@ -322,6 +319,21 @@
   </si>
   <si>
     <t>Page number based on each customer</t>
+  </si>
+  <si>
+    <t>6,7</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>TASK11</t>
+  </si>
+  <si>
+    <t>Dynamic Logo Change based on customer,page number</t>
+  </si>
+  <si>
+    <t>Limit record per page</t>
   </si>
 </sst>
 </file>
@@ -502,7 +514,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -568,6 +580,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -600,15 +615,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>107675</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>78441</xdr:rowOff>
+      <xdr:colOff>421442</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3898624</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>177545</xdr:rowOff>
+      <xdr:colOff>2935942</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>130274</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -624,7 +639,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -637,8 +652,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1441175" y="7720853"/>
-          <a:ext cx="3790949" cy="2004104"/>
+          <a:off x="1754942" y="10634383"/>
+          <a:ext cx="2514500" cy="1329303"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -650,15 +665,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>33619</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>75786</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>5915025</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>64649</xdr:rowOff>
+      <xdr:colOff>5715000</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>64648</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -673,7 +688,7 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
+      <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -681,14 +696,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect r="7960"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1504950" y="8562975"/>
-          <a:ext cx="5743575" cy="1407674"/>
+          <a:off x="1367119" y="7146698"/>
+          <a:ext cx="5681381" cy="1512862"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -958,9 +972,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G15"/>
+  <dimension ref="A2:G18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -1124,8 +1138,8 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="2">
-        <v>6</v>
+      <c r="A15" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="B15" s="3">
         <v>44375</v>
@@ -1135,6 +1149,39 @@
       </c>
       <c r="D15" s="2" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="2">
+        <v>8</v>
+      </c>
+      <c r="B16" s="24">
+        <v>44376</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2">
+        <v>9</v>
+      </c>
+      <c r="B17" s="24">
+        <v>44377</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="2">
+        <v>10</v>
+      </c>
+      <c r="B18" s="24">
+        <v>44377</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1147,8 +1194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1427,9 +1474,6 @@
       <c r="A38" s="21">
         <v>44375</v>
       </c>
-      <c r="B38" t="s">
-        <v>42</v>
-      </c>
       <c r="C38" s="1" t="s">
         <v>40</v>
       </c>
@@ -1437,17 +1481,11 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="21"/>
-      <c r="B39" t="s">
-        <v>41</v>
-      </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="21"/>
-      <c r="B40" s="22" t="s">
-        <v>66</v>
-      </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
     </row>
@@ -1502,17 +1540,23 @@
       <c r="D50" s="1"/>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="21"/>
+      <c r="A51" s="21">
+        <v>44375</v>
+      </c>
+      <c r="B51" t="s">
+        <v>42</v>
+      </c>
       <c r="D51" s="1"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="21"/>
+      <c r="B52" t="s">
+        <v>41</v>
+      </c>
       <c r="D52" s="1"/>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="21">
-        <v>44375</v>
-      </c>
+      <c r="A53" s="21"/>
       <c r="B53" s="22" t="s">
         <v>65</v>
       </c>
@@ -1530,6 +1574,9 @@
       <c r="A55" s="21">
         <v>44375</v>
       </c>
+      <c r="B55" s="22" t="s">
+        <v>64</v>
+      </c>
       <c r="C55" s="1" t="s">
         <v>44</v>
       </c>
@@ -1576,7 +1623,7 @@
         <v>57</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="D64" s="1"/>
     </row>
@@ -1593,7 +1640,7 @@
         <v>58</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D66" s="1"/>
     </row>
@@ -1610,7 +1657,7 @@
         <v>59</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D68" s="1"/>
     </row>
@@ -1626,7 +1673,7 @@
         <v>60</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:4">

</xml_diff>

<commit_message>
added task 11 files
</commit_message>
<xml_diff>
--- a/Work History.xlsx
+++ b/Work History.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7190" activeTab="1"/>
+    <workbookView windowWidth="18530" windowHeight="7190"/>
   </bookViews>
   <sheets>
     <sheet name="DAILY-TRACKER" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="86">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -128,7 +128,31 @@
     <t>Limit record per page</t>
   </si>
   <si>
-    <t xml:space="preserve">Table analysis - Important Fusion Tables </t>
+    <t>Table analysis - Important Fusion Tables, OTBI Analysis for all modules</t>
+  </si>
+  <si>
+    <t>Analysis OTBI</t>
+  </si>
+  <si>
+    <t>Analysis fsd and sales order tables</t>
+  </si>
+  <si>
+    <t>Analysed the FSD,table names and Links for Purchase orde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">task11-Working on PO tables report on Excel template </t>
+  </si>
+  <si>
+    <t>Kns cx training</t>
+  </si>
+  <si>
+    <t>11,12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analysis on BiP properties and report properties </t>
+  </si>
+  <si>
+    <t>task12-sql joins and set operators</t>
   </si>
   <si>
     <r>
@@ -322,28 +346,40 @@
     <t>TASK10</t>
   </si>
   <si>
+    <t>PO TABLE FROM CLIENT BASED REPORT PRACTICE</t>
+  </si>
+  <si>
+    <t>TASK11</t>
+  </si>
+  <si>
+    <t>IN-PROGRESS</t>
+  </si>
+  <si>
+    <t>SQL JOINS AND SET OPERATORS</t>
+  </si>
+  <si>
+    <t>TASK12</t>
+  </si>
+  <si>
     <t>Sales Order Details</t>
   </si>
   <si>
-    <t>TASK11</t>
+    <t>TASK13</t>
   </si>
   <si>
     <t>Purchase Order Details</t>
   </si>
   <si>
-    <t>TASK12</t>
+    <t>TASK14</t>
   </si>
   <si>
     <t>AR Aging Report</t>
   </si>
   <si>
-    <t>TASK13</t>
-  </si>
-  <si>
     <t>AP Aging Report</t>
   </si>
   <si>
-    <t>TASK14</t>
+    <t>TASK15</t>
   </si>
 </sst>
 </file>
@@ -351,12 +387,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="dd/mmm/yy"/>
-    <numFmt numFmtId="181" formatCode="[$-409]d/mmm/yyyy;@"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="[$-409]d/mmm/yyyy;@"/>
+    <numFmt numFmtId="181" formatCode="dd/mmm/yy"/>
     <numFmt numFmtId="182" formatCode="dd/mmm"/>
   </numFmts>
   <fonts count="27">
@@ -384,17 +420,60 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10.5"/>
       <color rgb="FF202124"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9.75"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -405,21 +484,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -434,14 +514,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -449,8 +521,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -464,9 +545,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -477,51 +557,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -563,7 +598,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -602,7 +637,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -620,31 +721,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -656,114 +793,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -771,12 +800,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -827,15 +850,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -847,6 +861,50 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -875,41 +933,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -927,150 +950,150 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1091,35 +1114,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1134,9 +1158,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1558,10 +1583,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:G19"/>
+  <dimension ref="A2:G22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13636363636364" defaultRowHeight="14.5" outlineLevelCol="6"/>
@@ -1585,19 +1610,19 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="21" t="s">
         <v>5</v>
       </c>
       <c r="F5"/>
@@ -1606,7 +1631,7 @@
       <c r="A7" s="9">
         <v>1</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="22">
         <v>44363</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -1624,10 +1649,10 @@
       <c r="A8" s="9">
         <v>2</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="22">
         <v>44364</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="22" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="9" t="s">
@@ -1638,7 +1663,7 @@
       <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="22">
         <v>44367</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -1653,7 +1678,7 @@
       <c r="A10" s="10">
         <v>1</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="22">
         <v>44368</v>
       </c>
       <c r="C10" s="9" t="s">
@@ -1667,7 +1692,7 @@
       <c r="A11" s="9">
         <v>3</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="22">
         <v>44369</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -1681,7 +1706,7 @@
       <c r="A12" s="9">
         <v>4</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="22">
         <v>44370</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -1695,13 +1720,13 @@
       <c r="A13" s="9">
         <v>5</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B13" s="22">
         <v>44371</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="24" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="9" t="s">
@@ -1712,7 +1737,7 @@
       <c r="A14" s="9">
         <v>6</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="22">
         <v>44373</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -1729,7 +1754,7 @@
       <c r="A15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="22">
         <v>44375</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -1743,7 +1768,7 @@
       <c r="A16" s="9">
         <v>8</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="22">
         <v>44376</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -1754,7 +1779,7 @@
       <c r="A17" s="9">
         <v>9</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="22">
         <v>44377</v>
       </c>
       <c r="C17" s="9" t="s">
@@ -1771,7 +1796,7 @@
       <c r="A18" s="9">
         <v>10</v>
       </c>
-      <c r="B18" s="21">
+      <c r="B18" s="22">
         <v>44377</v>
       </c>
       <c r="C18" s="9" t="s">
@@ -1788,16 +1813,67 @@
       <c r="A19" s="9">
         <v>11</v>
       </c>
-      <c r="B19" s="21">
+      <c r="B19" s="22">
         <v>44378</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E19" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="9">
+        <v>11</v>
+      </c>
+      <c r="B20" s="22">
+        <v>44379</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="9">
+        <v>11</v>
+      </c>
+      <c r="B21" s="22">
+        <v>44382</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="22">
+        <v>44383</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1811,10 +1887,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:D71"/>
+  <dimension ref="A2:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="3"/>
@@ -1828,41 +1904,41 @@
     <row r="2" ht="15.25"/>
     <row r="3" spans="2:2">
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" s="2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" ht="15.25" spans="2:2">
       <c r="B7" s="4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="5" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="3:3">
@@ -1882,10 +1958,10 @@
         <v>44363</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D14" s="11">
         <v>44368</v>
@@ -1896,10 +1972,10 @@
         <v>44364</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D15" s="11">
         <v>44365</v>
@@ -1910,7 +1986,7 @@
         <v>44368</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -1918,7 +1994,7 @@
     <row r="17" spans="1:4">
       <c r="A17" s="14"/>
       <c r="B17" s="13" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -1926,7 +2002,7 @@
     <row r="18" spans="1:4">
       <c r="A18" s="14"/>
       <c r="B18" s="13" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -1941,10 +2017,10 @@
         <v>44370</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D20" s="11">
         <v>44370</v>
@@ -1953,7 +2029,7 @@
     <row r="21" spans="1:4">
       <c r="A21" s="14"/>
       <c r="B21" s="15" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -1978,10 +2054,10 @@
         <v>44371</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D25" s="11">
         <v>44370</v>
@@ -1990,7 +2066,7 @@
     <row r="26" spans="1:4">
       <c r="A26" s="14"/>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1998,7 +2074,7 @@
     <row r="27" spans="1:4">
       <c r="A27" s="14"/>
       <c r="B27" s="15" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -2006,7 +2082,7 @@
     <row r="28" spans="1:4">
       <c r="A28" s="14"/>
       <c r="B28" s="15" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -2014,7 +2090,7 @@
     <row r="29" spans="1:4">
       <c r="A29" s="14"/>
       <c r="B29" s="15" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -2022,7 +2098,7 @@
     <row r="30" spans="1:4">
       <c r="A30" s="14"/>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -2037,10 +2113,10 @@
         <v>44371</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D32" s="11">
         <v>44374</v>
@@ -2059,7 +2135,7 @@
         <v>18</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D34" s="11">
         <v>44375</v>
@@ -2075,10 +2151,10 @@
         <v>44372</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D36" s="11">
         <v>44375</v>
@@ -2094,7 +2170,7 @@
         <v>44375</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D38" s="11">
         <v>44376</v>
@@ -2165,24 +2241,24 @@
         <v>44375</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D51" s="7"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="14"/>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="D52" s="7"/>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="14"/>
       <c r="B53" s="17" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D53" s="11">
         <v>44377</v>
@@ -2198,10 +2274,10 @@
         <v>44375</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D55" s="11">
         <v>44377</v>
@@ -2241,68 +2317,101 @@
       <c r="D63" s="7"/>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="14">
-        <v>44376</v>
-      </c>
-      <c r="B64" s="18" t="s">
-        <v>66</v>
+      <c r="A64" s="11">
+        <v>44382</v>
+      </c>
+      <c r="B64" t="s">
+        <v>74</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D64" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="14"/>
+      <c r="A65" s="18"/>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="14">
-        <v>44376</v>
-      </c>
-      <c r="B66" s="18" t="s">
-        <v>68</v>
+      <c r="A66" s="11">
+        <v>44382</v>
+      </c>
+      <c r="B66" t="s">
+        <v>77</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D66" s="7"/>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="14"/>
+        <v>78</v>
+      </c>
+      <c r="D66" s="11">
+        <v>44383</v>
+      </c>
+    </row>
+    <row r="67" spans="3:4">
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
     </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="14">
+    <row r="68" spans="4:4">
+      <c r="D68" s="7"/>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="14">
         <v>44376</v>
       </c>
-      <c r="B68" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D68" s="7"/>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="14"/>
-      <c r="C69" s="7"/>
+      <c r="B69" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="14">
+      <c r="A70" s="14"/>
+      <c r="C70" s="7"/>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="14">
         <v>44376</v>
       </c>
-      <c r="B70" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" s="14"/>
+      <c r="B71" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="14"/>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="14">
+        <v>44376</v>
+      </c>
+      <c r="B73" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="14"/>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="14">
+        <v>44376</v>
+      </c>
+      <c r="B75" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
added task 13 files
</commit_message>
<xml_diff>
--- a/Work History.xlsx
+++ b/Work History.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7190"/>
+    <workbookView windowWidth="18530" windowHeight="7190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DAILY-TRACKER" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="88">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>task12-sql joins and set operators</t>
+  </si>
+  <si>
+    <t>Muthukrishnan Session - SQL Functions &amp; Report Properties</t>
+  </si>
+  <si>
+    <t>Supplier Query Task (Muthukrishnan's Task)</t>
   </si>
   <si>
     <r>
@@ -361,25 +367,25 @@
     <t>TASK12</t>
   </si>
   <si>
+    <t>TASK 13</t>
+  </si>
+  <si>
+    <t>Customer Query Task (Muthukrishnan's Task)</t>
+  </si>
+  <si>
+    <t>TASK 14</t>
+  </si>
+  <si>
     <t>Sales Order Details</t>
   </si>
   <si>
-    <t>TASK13</t>
-  </si>
-  <si>
     <t>Purchase Order Details</t>
   </si>
   <si>
-    <t>TASK14</t>
-  </si>
-  <si>
     <t>AR Aging Report</t>
   </si>
   <si>
     <t>AP Aging Report</t>
-  </si>
-  <si>
-    <t>TASK15</t>
   </si>
 </sst>
 </file>
@@ -388,10 +394,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="[$-409]d/mmm/yyyy;@"/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="[$-409]d/mmm/yyyy;@"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="181" formatCode="dd/mmm/yy"/>
     <numFmt numFmtId="182" formatCode="dd/mmm"/>
   </numFmts>
@@ -433,13 +439,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -454,7 +453,60 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -469,6 +521,14 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -477,55 +537,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -538,21 +560,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -560,9 +567,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -631,175 +637,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -850,32 +856,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -900,6 +880,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -909,10 +904,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -932,168 +953,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1114,7 +1120,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1132,7 +1138,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1143,6 +1149,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1583,10 +1595,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:G22"/>
+  <dimension ref="A2:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13636363636364" defaultRowHeight="14.5" outlineLevelCol="6"/>
@@ -1610,19 +1622,19 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="23" t="s">
         <v>5</v>
       </c>
       <c r="F5"/>
@@ -1631,7 +1643,7 @@
       <c r="A7" s="9">
         <v>1</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="24">
         <v>44363</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -1649,10 +1661,10 @@
       <c r="A8" s="9">
         <v>2</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="24">
         <v>44364</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="24" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="9" t="s">
@@ -1663,7 +1675,7 @@
       <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="24">
         <v>44367</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -1678,7 +1690,7 @@
       <c r="A10" s="10">
         <v>1</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="24">
         <v>44368</v>
       </c>
       <c r="C10" s="9" t="s">
@@ -1692,7 +1704,7 @@
       <c r="A11" s="9">
         <v>3</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="24">
         <v>44369</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -1706,7 +1718,7 @@
       <c r="A12" s="9">
         <v>4</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="24">
         <v>44370</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -1720,13 +1732,13 @@
       <c r="A13" s="9">
         <v>5</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="24">
         <v>44371</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="26" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="9" t="s">
@@ -1737,7 +1749,7 @@
       <c r="A14" s="9">
         <v>6</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="24">
         <v>44373</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -1754,7 +1766,7 @@
       <c r="A15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="22">
+      <c r="B15" s="24">
         <v>44375</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -1768,7 +1780,7 @@
       <c r="A16" s="9">
         <v>8</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="24">
         <v>44376</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -1779,7 +1791,7 @@
       <c r="A17" s="9">
         <v>9</v>
       </c>
-      <c r="B17" s="22">
+      <c r="B17" s="24">
         <v>44377</v>
       </c>
       <c r="C17" s="9" t="s">
@@ -1796,7 +1808,7 @@
       <c r="A18" s="9">
         <v>10</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="24">
         <v>44377</v>
       </c>
       <c r="C18" s="9" t="s">
@@ -1813,7 +1825,7 @@
       <c r="A19" s="9">
         <v>11</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="24">
         <v>44378</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -1830,13 +1842,13 @@
       <c r="A20" s="9">
         <v>11</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="24">
         <v>44379</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="27" t="s">
         <v>30</v>
       </c>
       <c r="E20" s="9" t="s">
@@ -1847,7 +1859,7 @@
       <c r="A21" s="9">
         <v>11</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="24">
         <v>44382</v>
       </c>
       <c r="C21" s="9" t="s">
@@ -1864,7 +1876,7 @@
       <c r="A22" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="22">
+      <c r="B22" s="24">
         <v>44383</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -1874,6 +1886,23 @@
         <v>35</v>
       </c>
       <c r="E22" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="9">
+        <v>13</v>
+      </c>
+      <c r="B23" s="24">
+        <v>44384</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1887,10 +1916,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:D76"/>
+  <dimension ref="A2:D80"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="3"/>
@@ -1904,41 +1933,41 @@
     <row r="2" ht="15.25"/>
     <row r="3" spans="2:2">
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" ht="15.25" spans="2:2">
       <c r="B7" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="3:3">
@@ -1958,10 +1987,10 @@
         <v>44363</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D14" s="11">
         <v>44368</v>
@@ -1972,10 +2001,10 @@
         <v>44364</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D15" s="11">
         <v>44365</v>
@@ -1986,7 +2015,7 @@
         <v>44368</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -1994,7 +2023,7 @@
     <row r="17" spans="1:4">
       <c r="A17" s="14"/>
       <c r="B17" s="13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -2002,7 +2031,7 @@
     <row r="18" spans="1:4">
       <c r="A18" s="14"/>
       <c r="B18" s="13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -2017,10 +2046,10 @@
         <v>44370</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D20" s="11">
         <v>44370</v>
@@ -2029,7 +2058,7 @@
     <row r="21" spans="1:4">
       <c r="A21" s="14"/>
       <c r="B21" s="15" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -2054,10 +2083,10 @@
         <v>44371</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D25" s="11">
         <v>44370</v>
@@ -2066,7 +2095,7 @@
     <row r="26" spans="1:4">
       <c r="A26" s="14"/>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -2074,7 +2103,7 @@
     <row r="27" spans="1:4">
       <c r="A27" s="14"/>
       <c r="B27" s="15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -2082,7 +2111,7 @@
     <row r="28" spans="1:4">
       <c r="A28" s="14"/>
       <c r="B28" s="15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -2090,7 +2119,7 @@
     <row r="29" spans="1:4">
       <c r="A29" s="14"/>
       <c r="B29" s="15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -2098,7 +2127,7 @@
     <row r="30" spans="1:4">
       <c r="A30" s="14"/>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -2113,10 +2142,10 @@
         <v>44371</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D32" s="11">
         <v>44374</v>
@@ -2135,7 +2164,7 @@
         <v>18</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D34" s="11">
         <v>44375</v>
@@ -2151,10 +2180,10 @@
         <v>44372</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D36" s="11">
         <v>44375</v>
@@ -2170,7 +2199,7 @@
         <v>44375</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D38" s="11">
         <v>44376</v>
@@ -2241,24 +2270,24 @@
         <v>44375</v>
       </c>
       <c r="B51" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D51" s="7"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="14"/>
       <c r="B52" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D52" s="7"/>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="14"/>
       <c r="B53" s="17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D53" s="11">
         <v>44377</v>
@@ -2274,10 +2303,10 @@
         <v>44375</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D55" s="11">
         <v>44377</v>
@@ -2321,13 +2350,13 @@
         <v>44382</v>
       </c>
       <c r="B64" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2340,10 +2369,10 @@
         <v>44382</v>
       </c>
       <c r="B66" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D66" s="11">
         <v>44383</v>
@@ -2353,65 +2382,79 @@
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
     </row>
-    <row r="68" spans="4:4">
-      <c r="D68" s="7"/>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="14">
-        <v>44376</v>
-      </c>
-      <c r="B69" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>80</v>
+    <row r="68" spans="1:4">
+      <c r="A68" s="19">
+        <v>44383</v>
+      </c>
+      <c r="B68" t="s">
+        <v>37</v>
+      </c>
+      <c r="C68" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D68" s="11">
+        <v>44384</v>
       </c>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="14"/>
-      <c r="C70" s="7"/>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="14">
-        <v>44376</v>
-      </c>
-      <c r="B71" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="C71" s="7" t="s">
+      <c r="A70" s="19">
+        <v>44383</v>
+      </c>
+      <c r="B70" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" s="14"/>
+      <c r="C70" s="20" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="14">
         <v>44376</v>
       </c>
-      <c r="B73" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1">
+      <c r="B73" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C73" s="7"/>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74" s="14"/>
+      <c r="C74" s="7"/>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="14">
         <v>44376</v>
       </c>
-      <c r="B75" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="C75" s="7" t="s">
+      <c r="B75" s="21" t="s">
         <v>85</v>
       </c>
+      <c r="C75" s="7"/>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="14"/>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="14">
+        <v>44376</v>
+      </c>
+      <c r="B77" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C77" s="7"/>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="14"/>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="14">
+        <v>44376</v>
+      </c>
+      <c r="B79" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C79" s="7"/>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
added customer queries updated WorkHistory.xlsx
</commit_message>
<xml_diff>
--- a/Work History.xlsx
+++ b/Work History.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7190" activeTab="1"/>
+    <workbookView windowWidth="18530" windowHeight="7190"/>
   </bookViews>
   <sheets>
     <sheet name="DAILY-TRACKER" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="89">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>Supplier Query Task (Muthukrishnan's Task)</t>
+  </si>
+  <si>
+    <t>Muthukrishnan Session - SQL P2P session presented by Immanuel bro</t>
+  </si>
+  <si>
+    <t>SQL FUSION TABLE QUERIES(CUSTOMER)</t>
   </si>
   <si>
     <r>
@@ -373,9 +379,6 @@
     <t>Customer Query Task (Muthukrishnan's Task)</t>
   </si>
   <si>
-    <t>TASK 14</t>
-  </si>
-  <si>
     <t>Sales Order Details</t>
   </si>
   <si>
@@ -394,11 +397,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="[$-409]d/mmm/yyyy;@"/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="dd/mmm/yy"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="dd/mmm/yy"/>
+    <numFmt numFmtId="180" formatCode="[$-409]d/mmm/yyyy;@"/>
+    <numFmt numFmtId="181" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="182" formatCode="dd/mmm"/>
   </numFmts>
   <fonts count="27">
@@ -438,6 +441,29 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -445,15 +471,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -468,14 +488,68 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -489,86 +563,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -637,175 +640,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -859,45 +862,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -921,19 +885,34 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -953,153 +932,177 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1120,7 +1123,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1129,7 +1132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1138,7 +1141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1148,13 +1151,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1595,10 +1592,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:G23"/>
+  <dimension ref="A2:G24"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13636363636364" defaultRowHeight="14.5" outlineLevelCol="6"/>
@@ -1622,19 +1619,19 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="21" t="s">
         <v>5</v>
       </c>
       <c r="F5"/>
@@ -1643,7 +1640,7 @@
       <c r="A7" s="9">
         <v>1</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="22">
         <v>44363</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -1661,10 +1658,10 @@
       <c r="A8" s="9">
         <v>2</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="22">
         <v>44364</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="22" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="9" t="s">
@@ -1675,7 +1672,7 @@
       <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="22">
         <v>44367</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -1690,7 +1687,7 @@
       <c r="A10" s="10">
         <v>1</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="22">
         <v>44368</v>
       </c>
       <c r="C10" s="9" t="s">
@@ -1704,7 +1701,7 @@
       <c r="A11" s="9">
         <v>3</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="22">
         <v>44369</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -1718,7 +1715,7 @@
       <c r="A12" s="9">
         <v>4</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="22">
         <v>44370</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -1732,13 +1729,13 @@
       <c r="A13" s="9">
         <v>5</v>
       </c>
-      <c r="B13" s="24">
+      <c r="B13" s="22">
         <v>44371</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="24" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="9" t="s">
@@ -1749,7 +1746,7 @@
       <c r="A14" s="9">
         <v>6</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="22">
         <v>44373</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -1766,7 +1763,7 @@
       <c r="A15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="22">
         <v>44375</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -1780,7 +1777,7 @@
       <c r="A16" s="9">
         <v>8</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="22">
         <v>44376</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -1791,7 +1788,7 @@
       <c r="A17" s="9">
         <v>9</v>
       </c>
-      <c r="B17" s="24">
+      <c r="B17" s="22">
         <v>44377</v>
       </c>
       <c r="C17" s="9" t="s">
@@ -1808,7 +1805,7 @@
       <c r="A18" s="9">
         <v>10</v>
       </c>
-      <c r="B18" s="24">
+      <c r="B18" s="22">
         <v>44377</v>
       </c>
       <c r="C18" s="9" t="s">
@@ -1825,7 +1822,7 @@
       <c r="A19" s="9">
         <v>11</v>
       </c>
-      <c r="B19" s="24">
+      <c r="B19" s="22">
         <v>44378</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -1842,13 +1839,13 @@
       <c r="A20" s="9">
         <v>11</v>
       </c>
-      <c r="B20" s="24">
+      <c r="B20" s="22">
         <v>44379</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="D20" s="25" t="s">
         <v>30</v>
       </c>
       <c r="E20" s="9" t="s">
@@ -1859,7 +1856,7 @@
       <c r="A21" s="9">
         <v>11</v>
       </c>
-      <c r="B21" s="24">
+      <c r="B21" s="22">
         <v>44382</v>
       </c>
       <c r="C21" s="9" t="s">
@@ -1876,7 +1873,7 @@
       <c r="A22" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="24">
+      <c r="B22" s="22">
         <v>44383</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -1893,7 +1890,7 @@
       <c r="A23" s="9">
         <v>13</v>
       </c>
-      <c r="B23" s="24">
+      <c r="B23" s="22">
         <v>44384</v>
       </c>
       <c r="C23" s="9" t="s">
@@ -1903,6 +1900,23 @@
         <v>37</v>
       </c>
       <c r="E23" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="9">
+        <v>13</v>
+      </c>
+      <c r="B24" s="22">
+        <v>44385</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1918,7 +1932,7 @@
   <sheetPr/>
   <dimension ref="A2:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A54" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A63" workbookViewId="0">
       <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
@@ -1933,41 +1947,41 @@
     <row r="2" ht="15.25"/>
     <row r="3" spans="2:2">
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" ht="15.25" spans="2:2">
       <c r="B7" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="3:3">
@@ -1987,10 +2001,10 @@
         <v>44363</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D14" s="11">
         <v>44368</v>
@@ -2001,10 +2015,10 @@
         <v>44364</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D15" s="11">
         <v>44365</v>
@@ -2015,7 +2029,7 @@
         <v>44368</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -2023,7 +2037,7 @@
     <row r="17" spans="1:4">
       <c r="A17" s="14"/>
       <c r="B17" s="13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -2031,7 +2045,7 @@
     <row r="18" spans="1:4">
       <c r="A18" s="14"/>
       <c r="B18" s="13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -2046,10 +2060,10 @@
         <v>44370</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D20" s="11">
         <v>44370</v>
@@ -2058,7 +2072,7 @@
     <row r="21" spans="1:4">
       <c r="A21" s="14"/>
       <c r="B21" s="15" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -2083,10 +2097,10 @@
         <v>44371</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D25" s="11">
         <v>44370</v>
@@ -2095,7 +2109,7 @@
     <row r="26" spans="1:4">
       <c r="A26" s="14"/>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -2103,7 +2117,7 @@
     <row r="27" spans="1:4">
       <c r="A27" s="14"/>
       <c r="B27" s="15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -2111,7 +2125,7 @@
     <row r="28" spans="1:4">
       <c r="A28" s="14"/>
       <c r="B28" s="15" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -2119,7 +2133,7 @@
     <row r="29" spans="1:4">
       <c r="A29" s="14"/>
       <c r="B29" s="15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -2127,7 +2141,7 @@
     <row r="30" spans="1:4">
       <c r="A30" s="14"/>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -2142,10 +2156,10 @@
         <v>44371</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D32" s="11">
         <v>44374</v>
@@ -2164,7 +2178,7 @@
         <v>18</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D34" s="11">
         <v>44375</v>
@@ -2180,10 +2194,10 @@
         <v>44372</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D36" s="11">
         <v>44375</v>
@@ -2199,7 +2213,7 @@
         <v>44375</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D38" s="11">
         <v>44376</v>
@@ -2270,24 +2284,24 @@
         <v>44375</v>
       </c>
       <c r="B51" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D51" s="7"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="14"/>
       <c r="B52" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D52" s="7"/>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="14"/>
       <c r="B53" s="17" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D53" s="11">
         <v>44377</v>
@@ -2303,10 +2317,10 @@
         <v>44375</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D55" s="11">
         <v>44377</v>
@@ -2350,13 +2364,13 @@
         <v>44382</v>
       </c>
       <c r="B64" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2369,10 +2383,10 @@
         <v>44382</v>
       </c>
       <c r="B66" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D66" s="11">
         <v>44383</v>
@@ -2383,36 +2397,34 @@
       <c r="D67" s="7"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="19">
+      <c r="A68" s="11">
         <v>44383</v>
       </c>
       <c r="B68" t="s">
         <v>37</v>
       </c>
-      <c r="C68" s="20" t="s">
-        <v>81</v>
+      <c r="C68" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="D68" s="11">
         <v>44384</v>
       </c>
     </row>
+    <row r="69" spans="2:2">
+      <c r="B69" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="19">
-        <v>44383</v>
-      </c>
-      <c r="B70" t="s">
-        <v>82</v>
-      </c>
-      <c r="C70" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="A70" s="11"/>
+      <c r="C70" s="7"/>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="14">
         <v>44376</v>
       </c>
-      <c r="B73" s="21" t="s">
-        <v>84</v>
+      <c r="B73" s="19" t="s">
+        <v>85</v>
       </c>
       <c r="C73" s="7"/>
     </row>
@@ -2424,8 +2436,8 @@
       <c r="A75" s="14">
         <v>44376</v>
       </c>
-      <c r="B75" s="21" t="s">
-        <v>85</v>
+      <c r="B75" s="19" t="s">
+        <v>86</v>
       </c>
       <c r="C75" s="7"/>
     </row>
@@ -2436,8 +2448,8 @@
       <c r="A77" s="14">
         <v>44376</v>
       </c>
-      <c r="B77" s="21" t="s">
-        <v>86</v>
+      <c r="B77" s="19" t="s">
+        <v>87</v>
       </c>
       <c r="C77" s="7"/>
     </row>
@@ -2448,8 +2460,8 @@
       <c r="A79" s="14">
         <v>44376</v>
       </c>
-      <c r="B79" s="21" t="s">
-        <v>87</v>
+      <c r="B79" s="19" t="s">
+        <v>88</v>
       </c>
       <c r="C79" s="7"/>
     </row>

</xml_diff>

<commit_message>
added task 14 and task 15 folders
</commit_message>
<xml_diff>
--- a/Work History.xlsx
+++ b/Work History.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KAVINNARESHGR\Desktop\Fusion\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4691D304-0B49-4DB8-BA79-77C90008A5ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18525" windowHeight="7185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="18530" windowHeight="7190"/>
   </bookViews>
   <sheets>
     <sheet name="DAILY-TRACKER" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="100">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -171,6 +165,27 @@
   </si>
   <si>
     <t>SQL FUSION TABLE QUERIES(CUSTOMER)</t>
+  </si>
+  <si>
+    <t>11,13</t>
+  </si>
+  <si>
+    <t>SQL Queries and PO Datamodel  and Template ; Customer Muthu task</t>
+  </si>
+  <si>
+    <t>Column selector and View Selector in OTBI</t>
+  </si>
+  <si>
+    <t>Column selector &amp; View selector</t>
+  </si>
+  <si>
+    <t>Report properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report properties </t>
+  </si>
+  <si>
+    <t>Report properties Final Documentation</t>
   </si>
   <si>
     <r>
@@ -385,6 +400,18 @@
     <t>Customer Query Task (Muthukrishnan's Task)</t>
   </si>
   <si>
+    <t>View Selector &amp; Column Selector</t>
+  </si>
+  <si>
+    <t>TASK 14</t>
+  </si>
+  <si>
+    <t>Report Properties</t>
+  </si>
+  <si>
+    <t>TASK 15</t>
+  </si>
+  <si>
     <t>Sales Order Details</t>
   </si>
   <si>
@@ -395,42 +422,22 @@
   </si>
   <si>
     <t>AP Aging Report</t>
-  </si>
-  <si>
-    <t>Column selector and View Selector in OTBI</t>
-  </si>
-  <si>
-    <t>11,13</t>
-  </si>
-  <si>
-    <t>SQL Queries and PO Datamodel  and Template ; Customer Muthu task</t>
-  </si>
-  <si>
-    <t>View Selector &amp; Column Selector`</t>
-  </si>
-  <si>
-    <t>TASK 14</t>
-  </si>
-  <si>
-    <t>Report Properties</t>
-  </si>
-  <si>
-    <t>TASK 15</t>
-  </si>
-  <si>
-    <t>Report properties</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="dd/mmm/yy"/>
-    <numFmt numFmtId="165" formatCode="[$-409]d/mmm/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="dd/mmm"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="7">
+    <numFmt numFmtId="176" formatCode="[$-409]d/mmm/yyyy;@"/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="dd/mmm/yy"/>
+    <numFmt numFmtId="182" formatCode="dd/mmm"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,6 +474,142 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="5" tint="-0.499984740745262"/>
       <name val="Calibri"/>
@@ -497,7 +640,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -506,30 +649,216 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79992065187536243"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79995117038483843"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="0" tint="-0.0499893185216834"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799920651875362"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799951170384838"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -574,17 +903,256 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -600,7 +1168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -609,16 +1177,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -628,7 +1196,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -638,7 +1209,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -648,44 +1219,77 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFFFCC99"/>
-      <color rgb="FFFCF7CE"/>
-      <color rgb="FFFAD0E5"/>
-      <color rgb="FFD5D3F7"/>
+      <color rgb="00FFCC99"/>
+      <color rgb="00FCF7CE"/>
+      <color rgb="00FAD0E5"/>
+      <color rgb="00D5D3F7"/>
     </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -701,19 +1305,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -751,19 +1349,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1042,61 +1634,61 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A2:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.13636363636364" defaultRowHeight="14.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="9"/>
+    <col min="1" max="1" width="9.13636363636364" style="9"/>
     <col min="2" max="2" width="10" style="9" customWidth="1"/>
-    <col min="3" max="3" width="71.42578125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" style="9" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="9"/>
+    <col min="3" max="3" width="71.4272727272727" style="9" customWidth="1"/>
+    <col min="4" max="4" width="51.8545454545455" style="9" customWidth="1"/>
+    <col min="5" max="5" width="6.42727272727273" style="9" customWidth="1"/>
+    <col min="6" max="6" width="27.4272727272727" style="9" customWidth="1"/>
+    <col min="7" max="7" width="19.4272727272727" style="9" customWidth="1"/>
+    <col min="8" max="16384" width="9.13636363636364" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="2" spans="3:3">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="3:3">
       <c r="C3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:6">
+      <c r="A5" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="22" t="s">
         <v>5</v>
       </c>
       <c r="F5"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:6">
       <c r="A7" s="9">
         <v>1</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="23">
         <v>44363</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -1110,14 +1702,14 @@
       </c>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:5">
       <c r="A8" s="9">
         <v>2</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="23">
         <v>44364</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="9" t="s">
@@ -1128,7 +1720,7 @@
       <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="23">
         <v>44367</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -1139,11 +1731,11 @@
       </c>
       <c r="G9"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:5">
       <c r="A10" s="10">
         <v>1</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="23">
         <v>44368</v>
       </c>
       <c r="C10" s="9" t="s">
@@ -1153,11 +1745,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:5">
       <c r="A11" s="9">
         <v>3</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="23">
         <v>44369</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -1167,11 +1759,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:5">
       <c r="A12" s="9">
         <v>4</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="23">
         <v>44370</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -1181,28 +1773,28 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="105">
+    <row r="13" ht="101.5" spans="1:5">
       <c r="A13" s="9">
         <v>5</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="23">
         <v>44371</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="25" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:5">
       <c r="A14" s="9">
         <v>6</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="23">
         <v>44373</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -1215,11 +1807,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:4">
       <c r="A15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="22">
+      <c r="B15" s="23">
         <v>44375</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -1229,11 +1821,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:3">
       <c r="A16" s="9">
         <v>8</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="23">
         <v>44376</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -1244,7 +1836,7 @@
       <c r="A17" s="9">
         <v>9</v>
       </c>
-      <c r="B17" s="22">
+      <c r="B17" s="23">
         <v>44377</v>
       </c>
       <c r="C17" s="9" t="s">
@@ -1261,7 +1853,7 @@
       <c r="A18" s="9">
         <v>10</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="23">
         <v>44377</v>
       </c>
       <c r="C18" s="9" t="s">
@@ -1278,7 +1870,7 @@
       <c r="A19" s="9">
         <v>11</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="23">
         <v>44378</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -1295,13 +1887,13 @@
       <c r="A20" s="9">
         <v>11</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="23">
         <v>44379</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="26" t="s">
         <v>30</v>
       </c>
       <c r="E20" s="9" t="s">
@@ -1312,7 +1904,7 @@
       <c r="A21" s="9">
         <v>11</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="23">
         <v>44382</v>
       </c>
       <c r="C21" s="9" t="s">
@@ -1329,7 +1921,7 @@
       <c r="A22" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="22">
+      <c r="B22" s="23">
         <v>44383</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -1346,7 +1938,7 @@
       <c r="A23" s="9">
         <v>13</v>
       </c>
-      <c r="B23" s="22">
+      <c r="B23" s="23">
         <v>44384</v>
       </c>
       <c r="C23" s="9" t="s">
@@ -1363,7 +1955,7 @@
       <c r="A24" s="9">
         <v>13</v>
       </c>
-      <c r="B24" s="22">
+      <c r="B24" s="23">
         <v>44385</v>
       </c>
       <c r="C24" s="9" t="s">
@@ -1378,16 +1970,16 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B25" s="26">
+        <v>40</v>
+      </c>
+      <c r="B25" s="23">
         <v>44386</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>91</v>
+        <v>41</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>8</v>
@@ -1397,81 +1989,104 @@
       <c r="A26" s="9">
         <v>14</v>
       </c>
-      <c r="B26" s="26">
+      <c r="B26" s="23">
         <v>44389</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>96</v>
+        <v>43</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="9">
+        <v>15</v>
+      </c>
+      <c r="B27" s="23">
+        <v>44390</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:D84"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A2:D84"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="93.28515625" customWidth="1"/>
+    <col min="2" max="2" width="93.2818181818182" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.1363636363636" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4">
+    <row r="2" ht="15.25"/>
+    <row r="3" spans="2:2">
       <c r="B3" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
       <c r="B4" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
       <c r="B5" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
       <c r="B6" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" ht="15.25" spans="2:2">
       <c r="B7" s="4" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="5" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="3:3">
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="3:3">
       <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:4">
@@ -1485,10 +2100,10 @@
         <v>44363</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D14" s="11">
         <v>44368</v>
@@ -1499,10 +2114,10 @@
         <v>44364</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D15" s="11">
         <v>44365</v>
@@ -1513,7 +2128,7 @@
         <v>44368</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -1521,7 +2136,7 @@
     <row r="17" spans="1:4">
       <c r="A17" s="14"/>
       <c r="B17" s="13" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -1529,7 +2144,7 @@
     <row r="18" spans="1:4">
       <c r="A18" s="14"/>
       <c r="B18" s="13" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -1544,10 +2159,10 @@
         <v>44370</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D20" s="11">
         <v>44370</v>
@@ -1556,7 +2171,7 @@
     <row r="21" spans="1:4">
       <c r="A21" s="14"/>
       <c r="B21" s="15" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -1581,10 +2196,10 @@
         <v>44371</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D25" s="11">
         <v>44370</v>
@@ -1593,7 +2208,7 @@
     <row r="26" spans="1:4">
       <c r="A26" s="14"/>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1601,7 +2216,7 @@
     <row r="27" spans="1:4">
       <c r="A27" s="14"/>
       <c r="B27" s="15" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -1609,7 +2224,7 @@
     <row r="28" spans="1:4">
       <c r="A28" s="14"/>
       <c r="B28" s="15" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1617,7 +2232,7 @@
     <row r="29" spans="1:4">
       <c r="A29" s="14"/>
       <c r="B29" s="15" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1625,7 +2240,7 @@
     <row r="30" spans="1:4">
       <c r="A30" s="14"/>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -1640,10 +2255,10 @@
         <v>44371</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D32" s="11">
         <v>44374</v>
@@ -1662,7 +2277,7 @@
         <v>18</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="D34" s="11">
         <v>44375</v>
@@ -1678,10 +2293,10 @@
         <v>44372</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="D36" s="11">
         <v>44375</v>
@@ -1697,7 +2312,7 @@
         <v>44375</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D38" s="11">
         <v>44376</v>
@@ -1768,24 +2383,24 @@
         <v>44375</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="D51" s="7"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="14"/>
       <c r="B52" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="D52" s="7"/>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="14"/>
       <c r="B53" s="17" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="D53" s="11">
         <v>44377</v>
@@ -1801,10 +2416,10 @@
         <v>44375</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="D55" s="11">
         <v>44377</v>
@@ -1848,13 +2463,13 @@
         <v>44382</v>
       </c>
       <c r="B64" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1867,16 +2482,16 @@
         <v>44382</v>
       </c>
       <c r="B66" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D66" s="11">
         <v>44383</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="3:4">
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
     </row>
@@ -1888,23 +2503,23 @@
         <v>37</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="D68" s="11">
         <v>44384</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="2:2">
       <c r="B69" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70" s="11"/>
       <c r="C70" s="7"/>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="28">
+      <c r="A71" s="11">
         <v>44386</v>
       </c>
       <c r="B71" t="s">
@@ -1913,15 +2528,15 @@
       <c r="C71" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D71" s="29">
+      <c r="D71" s="19">
         <v>44386</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="3:3">
       <c r="C73" s="7"/>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="28">
+      <c r="A74" s="11">
         <v>44389</v>
       </c>
       <c r="B74" t="s">
@@ -1930,66 +2545,67 @@
       <c r="C74" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D74" s="27">
+      <c r="D74" s="18">
         <v>44390</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="3:3">
       <c r="C75" s="7"/>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:3">
       <c r="A77" s="14">
         <v>44376</v>
       </c>
-      <c r="B77" s="19" t="s">
-        <v>85</v>
+      <c r="B77" s="20" t="s">
+        <v>96</v>
       </c>
       <c r="C77" s="7"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:1">
       <c r="A78" s="14"/>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:3">
       <c r="A79" s="14">
         <v>44376</v>
       </c>
-      <c r="B79" s="19" t="s">
-        <v>86</v>
+      <c r="B79" s="20" t="s">
+        <v>97</v>
       </c>
       <c r="C79" s="7"/>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:1">
       <c r="A80" s="14"/>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="14">
         <v>44376</v>
       </c>
-      <c r="B81" s="19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
+      <c r="B81" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
       <c r="A82" s="14"/>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="14">
         <v>44376</v>
       </c>
-      <c r="B83" s="19" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
+      <c r="B83" s="20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
       <c r="A84" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId2" display="KAVINNARESH.RENGARAJ@CHAINSYS.COM"/>
+    <hyperlink ref="B5" r:id="rId3" display="HTTPS://WWW.GITHUB.COM/KAVINKAVIN16/FUSION"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>